<commit_message>
Corrected issue with rays pointing in the wrong direction
</commit_message>
<xml_diff>
--- a/RayCaster/docs/RayCaster Calcs v2.xlsx
+++ b/RayCaster/docs/RayCaster Calcs v2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://afdl-my.sharepoint.com/personal/grahame_white_apollo-fire_com/Documents/Documents/src/RayCaster/RayCaster/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://afdl-my.sharepoint.com/personal/grahame_white_apollo-fire_com/Documents/Desktop/RayCaster/RayCaster/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{586031CE-B6C3-442C-A271-31DD4C28437E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{586031CE-B6C3-442C-A271-31DD4C28437E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C752605B-49BE-4FF6-ABBA-5D1385F4E092}"/>
   <bookViews>
-    <workbookView xWindow="3795" yWindow="2550" windowWidth="21600" windowHeight="12735" xr2:uid="{5B6EEF75-9EB3-4904-881B-577D038E85DB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{5B6EEF75-9EB3-4904-881B-577D038E85DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -442,7 +442,8 @@
   <dimension ref="A1:G362"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <pane ySplit="2" topLeftCell="A181" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G183" sqref="G183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,40 +454,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="F1" s="2"/>
+      <c r="G1" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="2" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="1"/>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">

</xml_diff>